<commit_message>
Changes Made for FlipKart
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testData.xlsx
+++ b/src/test/resources/excel/testData.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vigneshs/Udemy-Channel/Selenium/Udemy-Selenium-Framework/src/test/resources/excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amalbari\ECommerce\Selenium-Advanced-Framework-Course\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17571113-A71D-2140-B7D4-4FA7E03BDA9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65439E6F-2F4B-427E-82CD-617BE231277D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16380" xr2:uid="{F1397648-29D4-0441-BEF2-D2F66028E387}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{F1397648-29D4-0441-BEF2-D2F66028E387}"/>
   </bookViews>
   <sheets>
-    <sheet name="Data" sheetId="1" r:id="rId1"/>
+    <sheet name="LoginTest" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,28 +34,66 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>username</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
-  <si>
-    <t>Admin</t>
-  </si>
-  <si>
-    <t>admin123</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+  <si>
+    <t>Verification</t>
+  </si>
+  <si>
+    <t>CorrectCredentials</t>
+  </si>
+  <si>
+    <t>InvalidEmailID</t>
+  </si>
+  <si>
+    <t>Test123</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>IncorrectPassword</t>
+  </si>
+  <si>
+    <t>EmptyEmailID</t>
+  </si>
+  <si>
+    <t>Test1</t>
+  </si>
+  <si>
+    <t>EmptyPassword</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>malbariamit006@gmail.com</t>
+  </si>
+  <si>
+    <t>Test007@gmail</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -78,13 +116,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -397,31 +439,92 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{462ADB19-0966-8547-9D82-BFF937FD29DF}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.125" customWidth="1"/>
+    <col min="2" max="2" width="19.875" customWidth="1"/>
+    <col min="3" max="3" width="24" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A6" r:id="rId1" display="malbariamit@gmail.com" xr:uid="{EBF90270-414A-4922-A22D-9EE4E6D131EC}"/>
+    <hyperlink ref="B6" r:id="rId2" display="Amit007@gmail" xr:uid="{76F5BF8D-FF0C-4B5F-BD35-15C1B4A1A920}"/>
+    <hyperlink ref="A3" r:id="rId3" display="malbariamit@gmail.com" xr:uid="{822D5E27-DB66-4F21-AD1E-37121AF68A4A}"/>
+    <hyperlink ref="A5" r:id="rId4" display="malbariamit@gmail.com" xr:uid="{EFE7DF6A-B76D-4616-9264-ED20CD4F3599}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>